<commit_message>
commit 6 Nov mrng
</commit_message>
<xml_diff>
--- a/EXCEL_OUPUT/YAU Stat Accts 31 Mar 2023 (signed).xlsx
+++ b/EXCEL_OUPUT/YAU Stat Accts 31 Mar 2023 (signed).xlsx
@@ -1797,13 +1797,13 @@
     <t>any lease incentives receivable;</t>
   </si>
   <si>
-    <t>certain to</t>
+    <t>to certain</t>
   </si>
   <si>
     <t>reflects the exercise of an option to</t>
   </si>
   <si>
-    <t>exercise to the options; and</t>
+    <t>to exercise the options; and</t>
   </si>
   <si>
     <t>rate at or</t>

</xml_diff>